<commit_message>
engineering module initial commit
</commit_message>
<xml_diff>
--- a/documentation/agent_subprocesses.xlsx
+++ b/documentation/agent_subprocesses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AguilarAJ15\Github\DMASpy\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA03EB4A-DB8D-419E-82C6-9B5010F6F2B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D652E521-F580-4E10-89AD-54928B825767}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8940" activeTab="1" xr2:uid="{CAC21F4D-DD05-433E-A4D1-511388D95AA3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8940" xr2:uid="{CAC21F4D-DD05-433E-A4D1-511388D95AA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Engineering Module" sheetId="1" r:id="rId1"/>
@@ -233,13 +233,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{765E7CB2-F713-4AA8-9E50-EE1A396F7A1C}">
   <dimension ref="A2:K10"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,13 +691,13 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -713,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF053229-67D3-4C65-B3CE-4AA87D0C030D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,16 +725,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>